<commit_message>
cambios de excel de git
</commit_message>
<xml_diff>
--- a/git_pruebas.xlsx
+++ b/git_pruebas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DAVICO\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{006BAA01-ADAA-470A-9EE6-B1BF208462AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9E033DC-0ABA-4D5E-B4CA-8322100503A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9450" yWindow="1065" windowWidth="22545" windowHeight="15285" xr2:uid="{16391890-2143-4509-82B1-4601F2316FB3}"/>
+    <workbookView xWindow="11265" yWindow="660" windowWidth="22545" windowHeight="15285" xr2:uid="{16391890-2143-4509-82B1-4601F2316FB3}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>github</t>
   </si>
@@ -110,6 +110,15 @@
   </si>
   <si>
     <t xml:space="preserve">descarga los ultimos cambios de la rama </t>
+  </si>
+  <si>
+    <t>primero se debe de clonar , luego se debe de hacer un checkout para poder ubicarnos en la rama ,luego creamos una rama local ,luego subimos la rama al git ,luego descargamos los ultimos cambios,lo demas ya dentro del software</t>
+  </si>
+  <si>
+    <t>git clone</t>
+  </si>
+  <si>
+    <t>orden opcional</t>
   </si>
 </sst>
 </file>
@@ -139,7 +148,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -162,14 +171,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -533,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0083D0F4-ECFA-4ADC-84C0-DFA24371F80F}">
-  <dimension ref="A1:B50"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,39 +578,51 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>18</v>
       </c>
@@ -595,7 +630,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>10</v>
       </c>
@@ -603,7 +638,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>12</v>
       </c>
@@ -611,7 +646,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>14</v>
       </c>
@@ -619,7 +654,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>16</v>
       </c>
@@ -627,11 +662,16 @@
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="B46" s="1"/>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>20</v>
       </c>
@@ -639,7 +679,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>22</v>
       </c>
@@ -647,20 +687,29 @@
         <v>23</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C49">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
     </row>
+    <row r="51" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>